<commit_message>
fix(data): Corregir FUENTE_DE_VERDAD.xlsx - Columnas ESTADO y CP sincronizadas
- ESTADO: 279 registros corregidos (MÉRIDA -> YUCATÁN)
- CP: 286 registros corregidos (códigos postales restaurados)
- Total: 565 correcciones basadas en archivo histórico
- Auditoría post-fix: 0 diferencias encontradas
- Documento: docs/AUDITORIA_FUENTE_VERDAD_17_ENE_2026.md
</commit_message>
<xml_diff>
--- a/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -610,13 +610,11 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M2" t="n">
+        <v>97138</v>
       </c>
       <c r="N2" t="inlineStr">
         <is>
@@ -699,13 +697,11 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M3" t="n">
+        <v>97138</v>
       </c>
       <c r="N3" t="inlineStr">
         <is>
@@ -788,13 +784,11 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M4" t="n">
+        <v>97138</v>
       </c>
       <c r="N4" t="inlineStr">
         <is>
@@ -877,13 +871,11 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M5" t="n">
+        <v>97138</v>
       </c>
       <c r="N5" t="inlineStr">
         <is>
@@ -966,13 +958,11 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M6" t="n">
+        <v>97138</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
@@ -1053,13 +1043,11 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M7" t="n">
+        <v>97138</v>
       </c>
       <c r="N7" t="inlineStr">
         <is>
@@ -1138,13 +1126,11 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M8" t="n">
+        <v>97138</v>
       </c>
       <c r="N8" t="inlineStr">
         <is>
@@ -1227,13 +1213,11 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M9" t="n">
+        <v>97138</v>
       </c>
       <c r="N9" t="inlineStr">
         <is>
@@ -1316,13 +1300,11 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M10" t="n">
+        <v>97138</v>
       </c>
       <c r="N10" t="inlineStr">
         <is>
@@ -1405,13 +1387,11 @@
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M11" t="n">
+        <v>97119</v>
       </c>
       <c r="N11" t="inlineStr">
         <is>
@@ -1492,13 +1472,11 @@
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M12" t="n">
+        <v>97119</v>
       </c>
       <c r="N12" t="inlineStr">
         <is>
@@ -1581,13 +1559,11 @@
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M13" t="n">
+        <v>97119</v>
       </c>
       <c r="N13" t="inlineStr">
         <is>
@@ -1670,13 +1646,11 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M14" t="n">
+        <v>97119</v>
       </c>
       <c r="N14" t="inlineStr">
         <is>
@@ -1759,13 +1733,11 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M15" t="n">
+        <v>97119</v>
       </c>
       <c r="N15" t="inlineStr">
         <is>
@@ -1844,13 +1816,11 @@
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M16" t="n">
+        <v>97119</v>
       </c>
       <c r="N16" t="inlineStr">
         <is>
@@ -1929,13 +1899,11 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M17" t="n">
+        <v>97119</v>
       </c>
       <c r="N17" t="inlineStr">
         <is>
@@ -2018,13 +1986,11 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M18" t="n">
+        <v>97119</v>
       </c>
       <c r="N18" t="inlineStr">
         <is>
@@ -2107,13 +2073,11 @@
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M19" t="n">
+        <v>97128</v>
       </c>
       <c r="N19" t="inlineStr">
         <is>
@@ -2196,13 +2160,11 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M20" t="n">
+        <v>97128</v>
       </c>
       <c r="N20" t="inlineStr">
         <is>
@@ -2285,13 +2247,11 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M21" t="n">
+        <v>97128</v>
       </c>
       <c r="N21" t="inlineStr">
         <is>
@@ -2374,13 +2334,11 @@
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M22" t="n">
+        <v>97128</v>
       </c>
       <c r="N22" t="inlineStr">
         <is>
@@ -2463,13 +2421,11 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M23" t="n">
+        <v>97128</v>
       </c>
       <c r="N23" t="inlineStr">
         <is>
@@ -2552,13 +2508,11 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M24" t="n">
+        <v>97128</v>
       </c>
       <c r="N24" t="inlineStr">
         <is>
@@ -2641,13 +2595,11 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M25" t="n">
+        <v>97128</v>
       </c>
       <c r="N25" t="inlineStr">
         <is>
@@ -2730,13 +2682,11 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M26" t="n">
+        <v>97128</v>
       </c>
       <c r="N26" t="inlineStr">
         <is>
@@ -2819,13 +2769,11 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M27" t="n">
+        <v>97128</v>
       </c>
       <c r="N27" t="inlineStr">
         <is>
@@ -2908,13 +2856,11 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M28" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M28" t="n">
+        <v>97128</v>
       </c>
       <c r="N28" t="inlineStr">
         <is>
@@ -2998,13 +2944,11 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M29" t="n">
+        <v>97960</v>
       </c>
       <c r="N29" t="inlineStr">
         <is>
@@ -3087,13 +3031,11 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M30" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M30" t="n">
+        <v>97960</v>
       </c>
       <c r="N30" t="inlineStr">
         <is>
@@ -3176,13 +3118,11 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M31" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M31" t="n">
+        <v>97960</v>
       </c>
       <c r="N31" t="inlineStr">
         <is>
@@ -3265,13 +3205,11 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M32" t="n">
+        <v>97960</v>
       </c>
       <c r="N32" t="inlineStr">
         <is>
@@ -3354,13 +3292,11 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M33" t="n">
+        <v>97960</v>
       </c>
       <c r="N33" t="inlineStr">
         <is>
@@ -3443,13 +3379,11 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M34" t="n">
+        <v>97200</v>
       </c>
       <c r="N34" t="inlineStr">
         <is>
@@ -3530,13 +3464,11 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M35" t="n">
+        <v>97200</v>
       </c>
       <c r="N35" t="inlineStr">
         <is>
@@ -3617,13 +3549,11 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M36" t="n">
+        <v>97200</v>
       </c>
       <c r="N36" t="inlineStr">
         <is>
@@ -3706,13 +3636,11 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M37" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M37" t="n">
+        <v>97200</v>
       </c>
       <c r="N37" t="inlineStr">
         <is>
@@ -3795,13 +3723,11 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M38" t="n">
+        <v>97200</v>
       </c>
       <c r="N38" t="inlineStr">
         <is>
@@ -3884,13 +3810,11 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M39" t="n">
+        <v>97200</v>
       </c>
       <c r="N39" t="inlineStr">
         <is>
@@ -3973,13 +3897,11 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M40" t="n">
+        <v>97200</v>
       </c>
       <c r="N40" t="inlineStr">
         <is>
@@ -4062,13 +3984,11 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M41" t="n">
+        <v>24115</v>
       </c>
       <c r="N41" t="inlineStr">
         <is>
@@ -4151,13 +4071,11 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M42" t="n">
+        <v>24115</v>
       </c>
       <c r="N42" t="inlineStr">
         <is>
@@ -4240,13 +4158,11 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M43" t="n">
+        <v>24115</v>
       </c>
       <c r="N43" t="inlineStr">
         <is>
@@ -4329,13 +4245,11 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M44" t="n">
+        <v>24115</v>
       </c>
       <c r="N44" t="inlineStr">
         <is>
@@ -4418,13 +4332,11 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M45" t="n">
+        <v>24115</v>
       </c>
       <c r="N45" t="inlineStr">
         <is>
@@ -4507,13 +4419,11 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M46" t="n">
+        <v>24115</v>
       </c>
       <c r="N46" t="inlineStr">
         <is>
@@ -4596,13 +4506,11 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M47" t="n">
+        <v>24115</v>
       </c>
       <c r="N47" t="inlineStr">
         <is>
@@ -4685,13 +4593,11 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M48" t="n">
+        <v>24115</v>
       </c>
       <c r="N48" t="inlineStr">
         <is>
@@ -4774,13 +4680,11 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M49" t="n">
+        <v>24115</v>
       </c>
       <c r="N49" t="inlineStr">
         <is>
@@ -4863,13 +4767,11 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>CARMEN</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M50" t="n">
+        <v>24115</v>
       </c>
       <c r="N50" t="inlineStr">
         <is>
@@ -4952,13 +4854,11 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M51" t="n">
+        <v>97138</v>
       </c>
       <c r="N51" t="inlineStr">
         <is>
@@ -5041,13 +4941,11 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M52" t="n">
+        <v>97138</v>
       </c>
       <c r="N52" t="inlineStr">
         <is>
@@ -5130,13 +5028,11 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M53" t="n">
+        <v>97138</v>
       </c>
       <c r="N53" t="inlineStr">
         <is>
@@ -5219,13 +5115,11 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M54" t="n">
+        <v>97138</v>
       </c>
       <c r="N54" t="inlineStr">
         <is>
@@ -5308,13 +5202,11 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M55" t="n">
+        <v>97143</v>
       </c>
       <c r="N55" t="inlineStr">
         <is>
@@ -5397,13 +5289,11 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M56" t="n">
+        <v>97143</v>
       </c>
       <c r="N56" t="inlineStr">
         <is>
@@ -5486,13 +5376,11 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M57" t="n">
+        <v>97143</v>
       </c>
       <c r="N57" t="inlineStr">
         <is>
@@ -5575,13 +5463,11 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M58" t="n">
+        <v>97143</v>
       </c>
       <c r="N58" t="inlineStr">
         <is>
@@ -5664,13 +5550,11 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M59" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M59" t="n">
+        <v>97143</v>
       </c>
       <c r="N59" t="inlineStr">
         <is>
@@ -5753,13 +5637,11 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M60" t="n">
+        <v>97143</v>
       </c>
       <c r="N60" t="inlineStr">
         <is>
@@ -5842,13 +5724,11 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M61" t="n">
+        <v>97308</v>
       </c>
       <c r="N61" t="inlineStr">
         <is>
@@ -5931,13 +5811,11 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M62" t="n">
+        <v>97308</v>
       </c>
       <c r="N62" t="inlineStr">
         <is>
@@ -6020,13 +5898,11 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M63" t="n">
+        <v>97308</v>
       </c>
       <c r="N63" t="inlineStr">
         <is>
@@ -6109,13 +5985,11 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M64" t="n">
+        <v>97308</v>
       </c>
       <c r="N64" t="inlineStr">
         <is>
@@ -6198,13 +6072,11 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M65" t="n">
+        <v>97308</v>
       </c>
       <c r="N65" t="inlineStr">
         <is>
@@ -6287,13 +6159,11 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M66" t="n">
+        <v>97308</v>
       </c>
       <c r="N66" t="inlineStr">
         <is>
@@ -6376,13 +6246,11 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M67" t="n">
+        <v>97308</v>
       </c>
       <c r="N67" t="inlineStr">
         <is>
@@ -6465,13 +6333,11 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M68" t="n">
+        <v>97308</v>
       </c>
       <c r="N68" t="inlineStr">
         <is>
@@ -6554,13 +6420,11 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M69" t="n">
+        <v>5120</v>
       </c>
       <c r="N69" t="inlineStr">
         <is>
@@ -6643,13 +6507,11 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M70" t="n">
+        <v>5120</v>
       </c>
       <c r="N70" t="inlineStr">
         <is>
@@ -6732,13 +6594,11 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M71" t="n">
+        <v>5120</v>
       </c>
       <c r="N71" t="inlineStr">
         <is>
@@ -6821,13 +6681,11 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M72" t="n">
+        <v>5120</v>
       </c>
       <c r="N72" t="inlineStr">
         <is>
@@ -6910,13 +6768,11 @@
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M73" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M73" t="n">
+        <v>5120</v>
       </c>
       <c r="N73" t="inlineStr">
         <is>
@@ -6999,13 +6855,11 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M74" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M74" t="n">
+        <v>5120</v>
       </c>
       <c r="N74" t="inlineStr">
         <is>
@@ -7088,13 +6942,11 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M75" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M75" t="n">
+        <v>5120</v>
       </c>
       <c r="N75" t="inlineStr">
         <is>
@@ -7177,13 +7029,11 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>MIGUEL HIDALGO</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr">
-        <is>
           <t>MÉXICO CDMX</t>
         </is>
+      </c>
+      <c r="M76" t="n">
+        <v>5120</v>
       </c>
       <c r="N76" t="inlineStr">
         <is>
@@ -7266,13 +7116,11 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>VALLADOLID</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M77" t="n">
+        <v>97780</v>
       </c>
       <c r="N77" t="inlineStr">
         <is>
@@ -7355,13 +7203,11 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>VALLADOLID</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M78" t="n">
+        <v>97780</v>
       </c>
       <c r="N78" t="inlineStr">
         <is>
@@ -7444,13 +7290,11 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>VALLADOLID</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M79" t="n">
+        <v>97780</v>
       </c>
       <c r="N79" t="inlineStr">
         <is>
@@ -7533,13 +7377,11 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>VALLADOLID</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M80" t="n">
+        <v>97780</v>
       </c>
       <c r="N80" t="inlineStr">
         <is>
@@ -7622,13 +7464,11 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M81" t="n">
+        <v>97130</v>
       </c>
       <c r="N81" t="inlineStr">
         <is>
@@ -7711,13 +7551,11 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M82" t="n">
+        <v>97130</v>
       </c>
       <c r="N82" t="inlineStr">
         <is>
@@ -7800,13 +7638,11 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M83" t="n">
+        <v>97130</v>
       </c>
       <c r="N83" t="inlineStr">
         <is>
@@ -7889,13 +7725,11 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M84" t="n">
+        <v>97210</v>
       </c>
       <c r="N84" t="inlineStr">
         <is>
@@ -7978,13 +7812,11 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M85" t="n">
+        <v>97210</v>
       </c>
       <c r="N85" t="inlineStr">
         <is>
@@ -8067,13 +7899,11 @@
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M86" t="n">
+        <v>97210</v>
       </c>
       <c r="N86" t="inlineStr">
         <is>
@@ -8156,13 +7986,11 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M87" t="n">
+        <v>97210</v>
       </c>
       <c r="N87" t="inlineStr">
         <is>
@@ -8245,13 +8073,11 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M88" t="n">
+        <v>97210</v>
       </c>
       <c r="N88" t="inlineStr">
         <is>
@@ -8334,13 +8160,11 @@
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M89" t="n">
+        <v>97134</v>
       </c>
       <c r="N89" t="inlineStr">
         <is>
@@ -8423,13 +8247,11 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M90" t="n">
+        <v>97134</v>
       </c>
       <c r="N90" t="inlineStr">
         <is>
@@ -8512,13 +8334,11 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M91" t="n">
+        <v>97134</v>
       </c>
       <c r="N91" t="inlineStr">
         <is>
@@ -8601,13 +8421,11 @@
       </c>
       <c r="L92" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M92" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M92" t="n">
+        <v>97134</v>
       </c>
       <c r="N92" t="inlineStr">
         <is>
@@ -8690,13 +8508,11 @@
       </c>
       <c r="L93" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M93" t="n">
+        <v>97215</v>
       </c>
       <c r="N93" t="inlineStr">
         <is>
@@ -8779,13 +8595,11 @@
       </c>
       <c r="L94" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M94" t="n">
+        <v>97215</v>
       </c>
       <c r="N94" t="inlineStr">
         <is>
@@ -8868,13 +8682,11 @@
       </c>
       <c r="L95" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M95" t="n">
+        <v>97215</v>
       </c>
       <c r="N95" t="inlineStr">
         <is>
@@ -8957,13 +8769,11 @@
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M96" t="n">
+        <v>97215</v>
       </c>
       <c r="N96" t="inlineStr">
         <is>
@@ -9046,13 +8856,11 @@
       </c>
       <c r="L97" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M97" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M97" t="n">
+        <v>97215</v>
       </c>
       <c r="N97" t="inlineStr">
         <is>
@@ -9135,13 +8943,11 @@
       </c>
       <c r="L98" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M98" t="n">
+        <v>97215</v>
       </c>
       <c r="N98" t="inlineStr">
         <is>
@@ -9224,13 +9030,11 @@
       </c>
       <c r="L99" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M99" t="n">
+        <v>97215</v>
       </c>
       <c r="N99" t="inlineStr">
         <is>
@@ -9313,13 +9117,11 @@
       </c>
       <c r="L100" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M100" t="n">
+        <v>97215</v>
       </c>
       <c r="N100" t="inlineStr">
         <is>
@@ -9402,13 +9204,11 @@
       </c>
       <c r="L101" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M101" t="n">
+        <v>97215</v>
       </c>
       <c r="N101" t="inlineStr">
         <is>
@@ -9491,13 +9291,11 @@
       </c>
       <c r="L102" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M102" t="n">
+        <v>97215</v>
       </c>
       <c r="N102" t="inlineStr">
         <is>
@@ -9580,13 +9378,11 @@
       </c>
       <c r="L103" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M103" t="n">
+        <v>97133</v>
       </c>
       <c r="N103" t="inlineStr">
         <is>
@@ -9669,13 +9465,11 @@
       </c>
       <c r="L104" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M104" t="n">
+        <v>97133</v>
       </c>
       <c r="N104" t="inlineStr">
         <is>
@@ -9758,13 +9552,11 @@
       </c>
       <c r="L105" t="inlineStr">
         <is>
-          <t>HECELCHAKÁN</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M105" t="n">
+        <v>24800</v>
       </c>
       <c r="N105" t="inlineStr">
         <is>
@@ -9845,13 +9637,11 @@
       </c>
       <c r="L106" t="inlineStr">
         <is>
-          <t>HECELCHAKÁN</t>
-        </is>
-      </c>
-      <c r="M106" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M106" t="n">
+        <v>24800</v>
       </c>
       <c r="N106" t="inlineStr">
         <is>
@@ -9932,13 +9722,11 @@
       </c>
       <c r="L107" t="inlineStr">
         <is>
-          <t>HECELCHAKÁN</t>
-        </is>
-      </c>
-      <c r="M107" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M107" t="n">
+        <v>24800</v>
       </c>
       <c r="N107" t="inlineStr">
         <is>
@@ -10019,13 +9807,11 @@
       </c>
       <c r="L108" t="inlineStr">
         <is>
-          <t>HECELCHAKÁN</t>
-        </is>
-      </c>
-      <c r="M108" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M108" t="n">
+        <v>24800</v>
       </c>
       <c r="N108" t="inlineStr">
         <is>
@@ -10111,10 +9897,8 @@
           <t>CAMPECHE</t>
         </is>
       </c>
-      <c r="M109" t="inlineStr">
-        <is>
-          <t>CAMPECHE</t>
-        </is>
+      <c r="M109" t="n">
+        <v>24085</v>
       </c>
       <c r="N109" t="inlineStr">
         <is>
@@ -10196,10 +9980,8 @@
           <t>CAMPECHE</t>
         </is>
       </c>
-      <c r="M110" t="inlineStr">
-        <is>
-          <t>CAMPECHE</t>
-        </is>
+      <c r="M110" t="n">
+        <v>24085</v>
       </c>
       <c r="N110" t="inlineStr">
         <is>
@@ -10283,10 +10065,8 @@
           <t>CAMPECHE</t>
         </is>
       </c>
-      <c r="M111" t="inlineStr">
-        <is>
-          <t>CAMPECHE</t>
-        </is>
+      <c r="M111" t="n">
+        <v>24085</v>
       </c>
       <c r="N111" t="inlineStr">
         <is>
@@ -10370,10 +10150,8 @@
           <t>CAMPECHE</t>
         </is>
       </c>
-      <c r="M112" t="inlineStr">
-        <is>
-          <t>CAMPECHE</t>
-        </is>
+      <c r="M112" t="n">
+        <v>24085</v>
       </c>
       <c r="N112" t="inlineStr">
         <is>
@@ -10459,10 +10237,8 @@
           <t>CAMPECHE</t>
         </is>
       </c>
-      <c r="M113" t="inlineStr">
-        <is>
-          <t>CAMPECHE</t>
-        </is>
+      <c r="M113" t="n">
+        <v>24085</v>
       </c>
       <c r="N113" t="inlineStr">
         <is>
@@ -10546,10 +10322,8 @@
           <t>CAMPECHE</t>
         </is>
       </c>
-      <c r="M114" t="inlineStr">
-        <is>
-          <t>CAMPECHE</t>
-        </is>
+      <c r="M114" t="n">
+        <v>24085</v>
       </c>
       <c r="N114" t="inlineStr">
         <is>
@@ -10632,13 +10406,11 @@
       </c>
       <c r="L115" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M115" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M115" t="n">
+        <v>97000</v>
       </c>
       <c r="N115" t="inlineStr">
         <is>
@@ -10721,13 +10493,11 @@
       </c>
       <c r="L116" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M116" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M116" t="n">
+        <v>97000</v>
       </c>
       <c r="N116" t="inlineStr">
         <is>
@@ -10810,13 +10580,11 @@
       </c>
       <c r="L117" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M117" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M117" t="n">
+        <v>97000</v>
       </c>
       <c r="N117" t="inlineStr">
         <is>
@@ -10899,13 +10667,11 @@
       </c>
       <c r="L118" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M118" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M118" t="n">
+        <v>97000</v>
       </c>
       <c r="N118" t="inlineStr">
         <is>
@@ -10988,13 +10754,11 @@
       </c>
       <c r="L119" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M119" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M119" t="n">
+        <v>97000</v>
       </c>
       <c r="N119" t="inlineStr">
         <is>
@@ -11077,13 +10841,11 @@
       </c>
       <c r="L120" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M120" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M120" t="n">
+        <v>97130</v>
       </c>
       <c r="N120" t="inlineStr">
         <is>
@@ -11166,13 +10928,11 @@
       </c>
       <c r="L121" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M121" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M121" t="n">
+        <v>97130</v>
       </c>
       <c r="N121" t="inlineStr">
         <is>
@@ -11255,13 +11015,11 @@
       </c>
       <c r="L122" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M122" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M122" t="n">
+        <v>97130</v>
       </c>
       <c r="N122" t="inlineStr">
         <is>
@@ -11344,13 +11102,11 @@
       </c>
       <c r="L123" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M123" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M123" t="n">
+        <v>97130</v>
       </c>
       <c r="N123" t="inlineStr">
         <is>
@@ -11433,13 +11189,11 @@
       </c>
       <c r="L124" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M124" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M124" t="n">
+        <v>97130</v>
       </c>
       <c r="N124" t="inlineStr">
         <is>
@@ -11522,13 +11276,11 @@
       </c>
       <c r="L125" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M125" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M125" t="n">
+        <v>97130</v>
       </c>
       <c r="N125" t="inlineStr">
         <is>
@@ -11611,13 +11363,11 @@
       </c>
       <c r="L126" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M126" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M126" t="n">
+        <v>97117</v>
       </c>
       <c r="N126" t="inlineStr">
         <is>
@@ -11698,13 +11448,11 @@
       </c>
       <c r="L127" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M127" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M127" t="n">
+        <v>97117</v>
       </c>
       <c r="N127" t="inlineStr">
         <is>
@@ -11787,13 +11535,11 @@
       </c>
       <c r="L128" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M128" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M128" t="n">
+        <v>97117</v>
       </c>
       <c r="N128" t="inlineStr">
         <is>
@@ -11876,13 +11622,11 @@
       </c>
       <c r="L129" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M129" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M129" t="n">
+        <v>97117</v>
       </c>
       <c r="N129" t="inlineStr">
         <is>
@@ -11963,13 +11707,11 @@
       </c>
       <c r="L130" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M130" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M130" t="n">
+        <v>97117</v>
       </c>
       <c r="N130" t="inlineStr">
         <is>
@@ -12052,13 +11794,11 @@
       </c>
       <c r="L131" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M131" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M131" t="n">
+        <v>97117</v>
       </c>
       <c r="N131" t="inlineStr">
         <is>
@@ -12141,13 +11881,11 @@
       </c>
       <c r="L132" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M132" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M132" t="n">
+        <v>97128</v>
       </c>
       <c r="N132" t="inlineStr">
         <is>
@@ -12230,13 +11968,11 @@
       </c>
       <c r="L133" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M133" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M133" t="n">
+        <v>97128</v>
       </c>
       <c r="N133" t="inlineStr">
         <is>
@@ -12319,13 +12055,11 @@
       </c>
       <c r="L134" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M134" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M134" t="n">
+        <v>97128</v>
       </c>
       <c r="N134" t="inlineStr">
         <is>
@@ -12406,13 +12140,11 @@
       </c>
       <c r="L135" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M135" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M135" t="n">
+        <v>97128</v>
       </c>
       <c r="N135" t="inlineStr">
         <is>
@@ -12495,13 +12227,11 @@
       </c>
       <c r="L136" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M136" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M136" t="n">
+        <v>97128</v>
       </c>
       <c r="N136" t="inlineStr">
         <is>
@@ -12584,13 +12314,11 @@
       </c>
       <c r="L137" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M137" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M137" t="n">
+        <v>97128</v>
       </c>
       <c r="N137" t="inlineStr">
         <is>
@@ -12673,13 +12401,11 @@
       </c>
       <c r="L138" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M138" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M138" t="n">
+        <v>97128</v>
       </c>
       <c r="N138" t="inlineStr">
         <is>
@@ -12760,13 +12486,11 @@
       </c>
       <c r="L139" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M139" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M139" t="n">
+        <v>97128</v>
       </c>
       <c r="N139" t="inlineStr">
         <is>
@@ -12847,13 +12571,11 @@
       </c>
       <c r="L140" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M140" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M140" t="n">
+        <v>97128</v>
       </c>
       <c r="N140" t="inlineStr">
         <is>
@@ -12934,13 +12656,11 @@
       </c>
       <c r="L141" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M141" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M141" t="n">
+        <v>97119</v>
       </c>
       <c r="N141" t="inlineStr">
         <is>
@@ -13021,13 +12741,11 @@
       </c>
       <c r="L142" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M142" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M142" t="n">
+        <v>97119</v>
       </c>
       <c r="N142" t="inlineStr">
         <is>
@@ -13108,13 +12826,11 @@
       </c>
       <c r="L143" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M143" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M143" t="n">
+        <v>97119</v>
       </c>
       <c r="N143" t="inlineStr">
         <is>
@@ -13197,13 +12913,11 @@
       </c>
       <c r="L144" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M144" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M144" t="n">
+        <v>97119</v>
       </c>
       <c r="N144" t="inlineStr">
         <is>
@@ -13286,13 +13000,11 @@
       </c>
       <c r="L145" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M145" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M145" t="n">
+        <v>97119</v>
       </c>
       <c r="N145" t="inlineStr">
         <is>
@@ -13375,13 +13087,11 @@
       </c>
       <c r="L146" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M146" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M146" t="n">
+        <v>97119</v>
       </c>
       <c r="N146" t="inlineStr">
         <is>
@@ -13464,13 +13174,11 @@
       </c>
       <c r="L147" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M147" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M147" t="n">
+        <v>97118</v>
       </c>
       <c r="N147" t="inlineStr">
         <is>
@@ -13549,13 +13257,11 @@
       </c>
       <c r="L148" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M148" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M148" t="n">
+        <v>97196</v>
       </c>
       <c r="N148" t="inlineStr">
         <is>
@@ -13638,13 +13344,11 @@
       </c>
       <c r="L149" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M149" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M149" t="n">
+        <v>97219</v>
       </c>
       <c r="N149" t="inlineStr">
         <is>
@@ -13729,13 +13433,11 @@
       </c>
       <c r="L150" t="inlineStr">
         <is>
-          <t>CANDELARIA</t>
-        </is>
-      </c>
-      <c r="M150" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M150" t="n">
+        <v>24330</v>
       </c>
       <c r="N150" t="inlineStr">
         <is>
@@ -13818,13 +13520,11 @@
       </c>
       <c r="L151" t="inlineStr">
         <is>
-          <t>CANDELARIA</t>
-        </is>
-      </c>
-      <c r="M151" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M151" t="n">
+        <v>24330</v>
       </c>
       <c r="N151" t="inlineStr">
         <is>
@@ -13909,13 +13609,11 @@
       </c>
       <c r="L152" t="inlineStr">
         <is>
-          <t>CANDELARIA</t>
-        </is>
-      </c>
-      <c r="M152" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M152" t="n">
+        <v>24330</v>
       </c>
       <c r="N152" t="inlineStr">
         <is>
@@ -14000,13 +13698,11 @@
       </c>
       <c r="L153" t="inlineStr">
         <is>
-          <t>CANDELARIA</t>
-        </is>
-      </c>
-      <c r="M153" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M153" t="n">
+        <v>24330</v>
       </c>
       <c r="N153" t="inlineStr">
         <is>
@@ -14087,13 +13783,11 @@
       </c>
       <c r="L154" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M154" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M154" t="n">
+        <v>97130</v>
       </c>
       <c r="N154" t="inlineStr">
         <is>
@@ -14176,13 +13870,11 @@
       </c>
       <c r="L155" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M155" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M155" t="n">
+        <v>97130</v>
       </c>
       <c r="N155" t="inlineStr">
         <is>
@@ -14265,13 +13957,11 @@
       </c>
       <c r="L156" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M156" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M156" t="n">
+        <v>97130</v>
       </c>
       <c r="N156" t="inlineStr">
         <is>
@@ -14352,13 +14042,11 @@
       </c>
       <c r="L157" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M157" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M157" t="n">
+        <v>97130</v>
       </c>
       <c r="N157" t="inlineStr">
         <is>
@@ -14441,13 +14129,11 @@
       </c>
       <c r="L158" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M158" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M158" t="n">
+        <v>97130</v>
       </c>
       <c r="N158" t="inlineStr">
         <is>
@@ -14530,13 +14216,11 @@
       </c>
       <c r="L159" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M159" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M159" t="n">
+        <v>97138</v>
       </c>
       <c r="N159" t="inlineStr">
         <is>
@@ -14617,13 +14301,11 @@
       </c>
       <c r="L160" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M160" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M160" t="n">
+        <v>97138</v>
       </c>
       <c r="N160" t="inlineStr">
         <is>
@@ -14704,13 +14386,11 @@
       </c>
       <c r="L161" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M161" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M161" t="n">
+        <v>97300</v>
       </c>
       <c r="N161" t="inlineStr">
         <is>
@@ -14793,13 +14473,11 @@
       </c>
       <c r="L162" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M162" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M162" t="n">
+        <v>97135</v>
       </c>
       <c r="N162" t="inlineStr">
         <is>
@@ -14882,13 +14560,11 @@
       </c>
       <c r="L163" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M163" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M163" t="n">
+        <v>97135</v>
       </c>
       <c r="N163" t="inlineStr">
         <is>
@@ -14971,13 +14647,11 @@
       </c>
       <c r="L164" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M164" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M164" t="n">
+        <v>97135</v>
       </c>
       <c r="N164" t="inlineStr">
         <is>
@@ -15060,13 +14734,11 @@
       </c>
       <c r="L165" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M165" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M165" t="n">
+        <v>97135</v>
       </c>
       <c r="N165" t="inlineStr">
         <is>
@@ -15149,13 +14821,11 @@
       </c>
       <c r="L166" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M166" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M166" t="n">
+        <v>97135</v>
       </c>
       <c r="N166" t="inlineStr">
         <is>
@@ -15238,13 +14908,11 @@
       </c>
       <c r="L167" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M167" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M167" t="n">
+        <v>97135</v>
       </c>
       <c r="N167" t="inlineStr">
         <is>
@@ -15327,13 +14995,11 @@
       </c>
       <c r="L168" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M168" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M168" t="n">
+        <v>97135</v>
       </c>
       <c r="N168" t="inlineStr">
         <is>
@@ -15416,13 +15082,11 @@
       </c>
       <c r="L169" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M169" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M169" t="n">
+        <v>97305</v>
       </c>
       <c r="N169" t="inlineStr">
         <is>
@@ -15505,13 +15169,11 @@
       </c>
       <c r="L170" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M170" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M170" t="n">
+        <v>97140</v>
       </c>
       <c r="N170" t="inlineStr">
         <is>
@@ -15594,13 +15256,11 @@
       </c>
       <c r="L171" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M171" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M171" t="n">
+        <v>97140</v>
       </c>
       <c r="N171" t="inlineStr">
         <is>
@@ -15681,13 +15341,11 @@
       </c>
       <c r="L172" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M172" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M172" t="n">
+        <v>97140</v>
       </c>
       <c r="N172" t="inlineStr">
         <is>
@@ -15770,13 +15428,11 @@
       </c>
       <c r="L173" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M173" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M173" t="n">
+        <v>97140</v>
       </c>
       <c r="N173" t="inlineStr">
         <is>
@@ -15859,13 +15515,11 @@
       </c>
       <c r="L174" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M174" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M174" t="n">
+        <v>97140</v>
       </c>
       <c r="N174" t="inlineStr">
         <is>
@@ -15948,13 +15602,11 @@
       </c>
       <c r="L175" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M175" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M175" t="n">
+        <v>97140</v>
       </c>
       <c r="N175" t="inlineStr">
         <is>
@@ -16037,13 +15689,11 @@
       </c>
       <c r="L176" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M176" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M176" t="n">
+        <v>97140</v>
       </c>
       <c r="N176" t="inlineStr">
         <is>
@@ -16126,13 +15776,11 @@
       </c>
       <c r="L177" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M177" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M177" t="n">
+        <v>97140</v>
       </c>
       <c r="N177" t="inlineStr">
         <is>
@@ -16213,13 +15861,11 @@
       </c>
       <c r="L178" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M178" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M178" t="n">
+        <v>97177</v>
       </c>
       <c r="N178" t="inlineStr">
         <is>
@@ -16302,13 +15948,11 @@
       </c>
       <c r="L179" t="inlineStr">
         <is>
-          <t>CAUCEL</t>
-        </is>
-      </c>
-      <c r="M179" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M179" t="n">
+        <v>97314</v>
       </c>
       <c r="N179" t="inlineStr">
         <is>
@@ -16389,13 +16033,11 @@
       </c>
       <c r="L180" t="inlineStr">
         <is>
-          <t>CAUCEL</t>
-        </is>
-      </c>
-      <c r="M180" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M180" t="n">
+        <v>97314</v>
       </c>
       <c r="N180" t="inlineStr">
         <is>
@@ -16478,13 +16120,11 @@
       </c>
       <c r="L181" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M181" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M181" t="n">
+        <v>97115</v>
       </c>
       <c r="N181" t="inlineStr">
         <is>
@@ -16565,13 +16205,11 @@
       </c>
       <c r="L182" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M182" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M182" t="n">
+        <v>97115</v>
       </c>
       <c r="N182" t="inlineStr">
         <is>
@@ -16654,13 +16292,11 @@
       </c>
       <c r="L183" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M183" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M183" t="n">
+        <v>97115</v>
       </c>
       <c r="N183" t="inlineStr">
         <is>
@@ -16739,13 +16375,11 @@
       </c>
       <c r="L184" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M184" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M184" t="n">
+        <v>97305</v>
       </c>
       <c r="N184" t="inlineStr">
         <is>
@@ -16826,13 +16460,11 @@
       </c>
       <c r="L185" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M185" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M185" t="n">
+        <v>97249</v>
       </c>
       <c r="N185" t="inlineStr">
         <is>
@@ -16915,13 +16547,11 @@
       </c>
       <c r="L186" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M186" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M186" t="n">
+        <v>97306</v>
       </c>
       <c r="N186" t="inlineStr">
         <is>
@@ -17004,13 +16634,11 @@
       </c>
       <c r="L187" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M187" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M187" t="n">
+        <v>97345</v>
       </c>
       <c r="N187" t="inlineStr">
         <is>
@@ -17093,13 +16721,11 @@
       </c>
       <c r="L188" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M188" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M188" t="n">
+        <v>97345</v>
       </c>
       <c r="N188" t="inlineStr">
         <is>
@@ -17182,13 +16808,11 @@
       </c>
       <c r="L189" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M189" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M189" t="n">
+        <v>97345</v>
       </c>
       <c r="N189" t="inlineStr">
         <is>
@@ -17271,13 +16895,11 @@
       </c>
       <c r="L190" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M190" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M190" t="n">
+        <v>97345</v>
       </c>
       <c r="N190" t="inlineStr">
         <is>
@@ -17360,13 +16982,11 @@
       </c>
       <c r="L191" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M191" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M191" t="n">
+        <v>97345</v>
       </c>
       <c r="N191" t="inlineStr">
         <is>
@@ -17449,13 +17069,11 @@
       </c>
       <c r="L192" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M192" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M192" t="n">
+        <v>97345</v>
       </c>
       <c r="N192" t="inlineStr">
         <is>
@@ -17538,13 +17156,11 @@
       </c>
       <c r="L193" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M193" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M193" t="n">
+        <v>97345</v>
       </c>
       <c r="N193" t="inlineStr">
         <is>
@@ -17627,13 +17243,11 @@
       </c>
       <c r="L194" t="inlineStr">
         <is>
-          <t>CONKAL</t>
-        </is>
-      </c>
-      <c r="M194" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M194" t="n">
+        <v>97345</v>
       </c>
       <c r="N194" t="inlineStr">
         <is>
@@ -17714,13 +17328,11 @@
       </c>
       <c r="L195" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M195" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M195" t="n">
+        <v>97970</v>
       </c>
       <c r="N195" t="inlineStr">
         <is>
@@ -17803,13 +17415,11 @@
       </c>
       <c r="L196" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M196" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M196" t="n">
+        <v>97970</v>
       </c>
       <c r="N196" t="inlineStr">
         <is>
@@ -17892,13 +17502,11 @@
       </c>
       <c r="L197" t="inlineStr">
         <is>
-          <t>TEKAX</t>
-        </is>
-      </c>
-      <c r="M197" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M197" t="n">
+        <v>97970</v>
       </c>
       <c r="N197" t="inlineStr">
         <is>
@@ -17981,13 +17589,11 @@
       </c>
       <c r="L198" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M198" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M198" t="n">
+        <v>97146</v>
       </c>
       <c r="N198" t="inlineStr">
         <is>
@@ -18070,13 +17676,11 @@
       </c>
       <c r="L199" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M199" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M199" t="n">
+        <v>97146</v>
       </c>
       <c r="N199" t="inlineStr">
         <is>
@@ -18157,13 +17761,11 @@
       </c>
       <c r="L200" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M200" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M200" t="n">
+        <v>97146</v>
       </c>
       <c r="N200" t="inlineStr">
         <is>
@@ -18246,13 +17848,11 @@
       </c>
       <c r="L201" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M201" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M201" t="n">
+        <v>97146</v>
       </c>
       <c r="N201" t="inlineStr">
         <is>
@@ -18335,13 +17935,11 @@
       </c>
       <c r="L202" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M202" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M202" t="n">
+        <v>97130</v>
       </c>
       <c r="N202" t="inlineStr">
         <is>
@@ -18424,13 +18022,11 @@
       </c>
       <c r="L203" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M203" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M203" t="n">
+        <v>97130</v>
       </c>
       <c r="N203" t="inlineStr">
         <is>
@@ -18513,13 +18109,11 @@
       </c>
       <c r="L204" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M204" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M204" t="n">
+        <v>97130</v>
       </c>
       <c r="N204" t="inlineStr">
         <is>
@@ -18600,13 +18194,11 @@
       </c>
       <c r="L205" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M205" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M205" t="n">
+        <v>97130</v>
       </c>
       <c r="N205" t="inlineStr">
         <is>
@@ -18689,13 +18281,11 @@
       </c>
       <c r="L206" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M206" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M206" t="n">
+        <v>97130</v>
       </c>
       <c r="N206" t="inlineStr">
         <is>
@@ -18778,13 +18368,11 @@
       </c>
       <c r="L207" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M207" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M207" t="n">
+        <v>97306</v>
       </c>
       <c r="N207" t="inlineStr">
         <is>
@@ -18867,13 +18455,11 @@
       </c>
       <c r="L208" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M208" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M208" t="n">
+        <v>97306</v>
       </c>
       <c r="N208" t="inlineStr">
         <is>
@@ -18956,13 +18542,11 @@
       </c>
       <c r="L209" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M209" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M209" t="n">
+        <v>97306</v>
       </c>
       <c r="N209" t="inlineStr">
         <is>
@@ -19045,13 +18629,11 @@
       </c>
       <c r="L210" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M210" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M210" t="n">
+        <v>97306</v>
       </c>
       <c r="N210" t="inlineStr">
         <is>
@@ -19134,13 +18716,11 @@
       </c>
       <c r="L211" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M211" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M211" t="n">
+        <v>97306</v>
       </c>
       <c r="N211" t="inlineStr">
         <is>
@@ -19223,13 +18803,11 @@
       </c>
       <c r="L212" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M212" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M212" t="n">
+        <v>97306</v>
       </c>
       <c r="N212" t="inlineStr">
         <is>
@@ -19312,13 +18890,11 @@
       </c>
       <c r="L213" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M213" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M213" t="n">
+        <v>97300</v>
       </c>
       <c r="N213" t="inlineStr">
         <is>
@@ -19401,13 +18977,11 @@
       </c>
       <c r="L214" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M214" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M214" t="n">
+        <v>97300</v>
       </c>
       <c r="N214" t="inlineStr">
         <is>
@@ -19490,13 +19064,11 @@
       </c>
       <c r="L215" t="inlineStr">
         <is>
-          <t>YUCATÁN</t>
-        </is>
-      </c>
-      <c r="M215" t="inlineStr">
-        <is>
           <t>MÉXICO</t>
         </is>
+      </c>
+      <c r="M215" t="n">
+        <v>97217</v>
       </c>
       <c r="N215" t="inlineStr">
         <is>
@@ -19554,13 +19126,11 @@
       </c>
       <c r="L216" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M216" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M216" t="n">
+        <v>97305</v>
       </c>
       <c r="N216" t="inlineStr">
         <is>
@@ -19641,13 +19211,11 @@
       </c>
       <c r="L217" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M217" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M217" t="n">
+        <v>97305</v>
       </c>
       <c r="N217" t="inlineStr">
         <is>
@@ -19730,13 +19298,11 @@
       </c>
       <c r="L218" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M218" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M218" t="n">
+        <v>97305</v>
       </c>
       <c r="N218" t="inlineStr">
         <is>
@@ -19819,13 +19385,11 @@
       </c>
       <c r="L219" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M219" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M219" t="n">
+        <v>97305</v>
       </c>
       <c r="N219" t="inlineStr">
         <is>
@@ -19906,13 +19470,11 @@
       </c>
       <c r="L220" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M220" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M220" t="n">
+        <v>97305</v>
       </c>
       <c r="N220" t="inlineStr">
         <is>
@@ -19995,13 +19557,11 @@
       </c>
       <c r="L221" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M221" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M221" t="n">
+        <v>97305</v>
       </c>
       <c r="N221" t="inlineStr">
         <is>
@@ -20084,13 +19644,11 @@
       </c>
       <c r="L222" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M222" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M222" t="n">
+        <v>97305</v>
       </c>
       <c r="N222" t="inlineStr">
         <is>
@@ -20173,13 +19731,11 @@
       </c>
       <c r="L223" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M223" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M223" t="n">
+        <v>97305</v>
       </c>
       <c r="N223" t="inlineStr">
         <is>
@@ -20262,13 +19818,11 @@
       </c>
       <c r="L224" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M224" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M224" t="n">
+        <v>97305</v>
       </c>
       <c r="N224" t="inlineStr">
         <is>
@@ -20351,13 +19905,11 @@
       </c>
       <c r="L225" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M225" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M225" t="n">
+        <v>97305</v>
       </c>
       <c r="N225" t="inlineStr">
         <is>
@@ -20440,13 +19992,11 @@
       </c>
       <c r="L226" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M226" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M226" t="n">
+        <v>97305</v>
       </c>
       <c r="N226" t="inlineStr">
         <is>
@@ -20529,13 +20079,11 @@
       </c>
       <c r="L227" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M227" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M227" t="n">
+        <v>97115</v>
       </c>
       <c r="N227" t="inlineStr">
         <is>
@@ -20616,13 +20164,11 @@
       </c>
       <c r="L228" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M228" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M228" t="n">
+        <v>97115</v>
       </c>
       <c r="N228" t="inlineStr">
         <is>
@@ -20705,13 +20251,11 @@
       </c>
       <c r="L229" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M229" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M229" t="n">
+        <v>97115</v>
       </c>
       <c r="N229" t="inlineStr">
         <is>
@@ -20794,13 +20338,11 @@
       </c>
       <c r="L230" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M230" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M230" t="n">
+        <v>97302</v>
       </c>
       <c r="N230" t="inlineStr">
         <is>
@@ -20861,10 +20403,8 @@
           <t>CAMPECHE</t>
         </is>
       </c>
-      <c r="M231" t="inlineStr">
-        <is>
-          <t>CAMPECHE</t>
-        </is>
+      <c r="M231" t="n">
+        <v>24085</v>
       </c>
       <c r="N231" t="inlineStr">
         <is>
@@ -20947,13 +20487,11 @@
       </c>
       <c r="L232" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M232" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M232" t="n">
+        <v>97302</v>
       </c>
       <c r="N232" t="inlineStr">
         <is>
@@ -21036,13 +20574,11 @@
       </c>
       <c r="L233" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M233" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M233" t="n">
+        <v>97302</v>
       </c>
       <c r="N233" t="inlineStr">
         <is>
@@ -21125,13 +20661,11 @@
       </c>
       <c r="L234" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M234" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M234" t="n">
+        <v>97302</v>
       </c>
       <c r="N234" t="inlineStr">
         <is>
@@ -21214,13 +20748,11 @@
       </c>
       <c r="L235" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M235" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M235" t="n">
+        <v>97302</v>
       </c>
       <c r="N235" t="inlineStr">
         <is>
@@ -21303,13 +20835,11 @@
       </c>
       <c r="L236" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M236" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M236" t="n">
+        <v>97302</v>
       </c>
       <c r="N236" t="inlineStr">
         <is>
@@ -21392,13 +20922,11 @@
       </c>
       <c r="L237" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M237" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M237" t="n">
+        <v>97302</v>
       </c>
       <c r="N237" t="inlineStr">
         <is>
@@ -21481,13 +21009,11 @@
       </c>
       <c r="L238" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M238" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M238" t="n">
+        <v>97314</v>
       </c>
       <c r="N238" t="inlineStr">
         <is>
@@ -21570,13 +21096,11 @@
       </c>
       <c r="L239" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M239" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M239" t="n">
+        <v>97314</v>
       </c>
       <c r="N239" t="inlineStr">
         <is>
@@ -21659,13 +21183,11 @@
       </c>
       <c r="L240" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M240" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M240" t="n">
+        <v>97314</v>
       </c>
       <c r="N240" t="inlineStr">
         <is>
@@ -21748,13 +21270,11 @@
       </c>
       <c r="L241" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M241" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M241" t="n">
+        <v>97145</v>
       </c>
       <c r="N241" t="inlineStr">
         <is>
@@ -21837,13 +21357,11 @@
       </c>
       <c r="L242" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M242" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M242" t="n">
+        <v>97145</v>
       </c>
       <c r="N242" t="inlineStr">
         <is>
@@ -21926,13 +21444,11 @@
       </c>
       <c r="L243" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M243" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M243" t="n">
+        <v>97145</v>
       </c>
       <c r="N243" t="inlineStr">
         <is>
@@ -22013,13 +21529,11 @@
       </c>
       <c r="L244" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M244" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M244" t="n">
+        <v>97302</v>
       </c>
       <c r="N244" t="inlineStr">
         <is>
@@ -22102,13 +21616,11 @@
       </c>
       <c r="L245" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M245" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M245" t="n">
+        <v>97314</v>
       </c>
       <c r="N245" t="inlineStr">
         <is>
@@ -22166,13 +21678,11 @@
       </c>
       <c r="L246" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M246" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M246" t="n">
+        <v>97130</v>
       </c>
       <c r="N246" t="inlineStr">
         <is>
@@ -22255,13 +21765,11 @@
       </c>
       <c r="L247" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M247" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M247" t="n">
+        <v>97130</v>
       </c>
       <c r="N247" t="inlineStr">
         <is>
@@ -22344,13 +21852,11 @@
       </c>
       <c r="L248" t="inlineStr">
         <is>
-          <t>Ciudad del Carmen</t>
-        </is>
-      </c>
-      <c r="M248" t="inlineStr">
-        <is>
           <t>CAMPECHE</t>
         </is>
+      </c>
+      <c r="M248" t="n">
+        <v>24114</v>
       </c>
       <c r="N248" t="inlineStr">
         <is>
@@ -22408,13 +21914,11 @@
       </c>
       <c r="L249" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M249" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M249" t="n">
+        <v>97117</v>
       </c>
       <c r="N249" t="inlineStr">
         <is>
@@ -22497,13 +22001,11 @@
       </c>
       <c r="L250" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M250" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M250" t="n">
+        <v>97117</v>
       </c>
       <c r="N250" t="inlineStr">
         <is>
@@ -22586,13 +22088,11 @@
       </c>
       <c r="L251" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M251" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M251" t="n">
+        <v>97117</v>
       </c>
       <c r="N251" t="inlineStr">
         <is>
@@ -22673,13 +22173,11 @@
       </c>
       <c r="L252" t="inlineStr">
         <is>
-          <t>Tizimín</t>
-        </is>
-      </c>
-      <c r="M252" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M252" t="n">
+        <v>97700</v>
       </c>
       <c r="N252" t="inlineStr">
         <is>
@@ -22739,13 +22237,11 @@
       </c>
       <c r="L253" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M253" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M253" t="n">
+        <v>97147</v>
       </c>
       <c r="N253" t="inlineStr">
         <is>
@@ -22830,13 +22326,11 @@
       </c>
       <c r="L254" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M254" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M254" t="n">
+        <v>97147</v>
       </c>
       <c r="N254" t="inlineStr">
         <is>
@@ -22921,13 +22415,11 @@
       </c>
       <c r="L255" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M255" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M255" t="n">
+        <v>97147</v>
       </c>
       <c r="N255" t="inlineStr">
         <is>
@@ -23012,13 +22504,11 @@
       </c>
       <c r="L256" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M256" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M256" t="n">
+        <v>97147</v>
       </c>
       <c r="N256" t="inlineStr">
         <is>
@@ -23103,13 +22593,11 @@
       </c>
       <c r="L257" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M257" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M257" t="n">
+        <v>97147</v>
       </c>
       <c r="N257" t="inlineStr">
         <is>
@@ -23194,13 +22682,11 @@
       </c>
       <c r="L258" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M258" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M258" t="n">
+        <v>97147</v>
       </c>
       <c r="N258" t="inlineStr">
         <is>
@@ -23285,13 +22771,11 @@
       </c>
       <c r="L259" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M259" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M259" t="n">
+        <v>97147</v>
       </c>
       <c r="N259" t="inlineStr">
         <is>
@@ -23374,13 +22858,11 @@
       </c>
       <c r="L260" t="inlineStr">
         <is>
-          <t>CHOCHOLA</t>
-        </is>
-      </c>
-      <c r="M260" t="inlineStr">
-        <is>
           <t>YUCATAN</t>
         </is>
+      </c>
+      <c r="M260" t="n">
+        <v>97816</v>
       </c>
       <c r="N260" t="inlineStr">
         <is>
@@ -23463,13 +22945,11 @@
       </c>
       <c r="L261" t="inlineStr">
         <is>
-          <t>CHOCHOLA</t>
-        </is>
-      </c>
-      <c r="M261" t="inlineStr">
-        <is>
           <t>YUCATAN</t>
         </is>
+      </c>
+      <c r="M261" t="n">
+        <v>97816</v>
       </c>
       <c r="N261" t="inlineStr">
         <is>
@@ -23552,13 +23032,11 @@
       </c>
       <c r="L262" t="inlineStr">
         <is>
-          <t>CHOCHOLA</t>
-        </is>
-      </c>
-      <c r="M262" t="inlineStr">
-        <is>
           <t>YUCATAN</t>
         </is>
+      </c>
+      <c r="M262" t="n">
+        <v>97816</v>
       </c>
       <c r="N262" t="inlineStr">
         <is>
@@ -23643,13 +23121,11 @@
       </c>
       <c r="L263" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M263" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M263" t="n">
+        <v>97205</v>
       </c>
       <c r="N263" t="inlineStr">
         <is>
@@ -23732,13 +23208,11 @@
       </c>
       <c r="L264" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M264" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M264" t="n">
+        <v>97205</v>
       </c>
       <c r="N264" t="inlineStr">
         <is>
@@ -23823,13 +23297,11 @@
       </c>
       <c r="L265" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M265" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M265" t="n">
+        <v>97205</v>
       </c>
       <c r="N265" t="inlineStr">
         <is>
@@ -23914,13 +23386,11 @@
       </c>
       <c r="L266" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M266" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M266" t="n">
+        <v>97205</v>
       </c>
       <c r="N266" t="inlineStr">
         <is>
@@ -24005,13 +23475,11 @@
       </c>
       <c r="L267" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M267" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M267" t="n">
+        <v>97205</v>
       </c>
       <c r="N267" t="inlineStr">
         <is>
@@ -24096,13 +23564,11 @@
       </c>
       <c r="L268" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M268" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M268" t="n">
+        <v>97205</v>
       </c>
       <c r="N268" t="inlineStr">
         <is>
@@ -24187,13 +23653,11 @@
       </c>
       <c r="L269" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M269" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M269" t="n">
+        <v>97205</v>
       </c>
       <c r="N269" t="inlineStr">
         <is>
@@ -24276,13 +23740,11 @@
       </c>
       <c r="L270" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M270" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M270" t="n">
+        <v>97302</v>
       </c>
       <c r="N270" t="inlineStr">
         <is>
@@ -24340,13 +23802,11 @@
       </c>
       <c r="L271" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M271" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M271" t="n">
+        <v>97305</v>
       </c>
       <c r="N271" t="inlineStr">
         <is>
@@ -24429,13 +23889,11 @@
       </c>
       <c r="L272" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M272" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M272" t="n">
+        <v>97305</v>
       </c>
       <c r="N272" t="inlineStr">
         <is>
@@ -24518,13 +23976,11 @@
       </c>
       <c r="L273" t="inlineStr">
         <is>
-          <t>MÉRIDA</t>
-        </is>
-      </c>
-      <c r="M273" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M273" t="n">
+        <v>97305</v>
       </c>
       <c r="N273" t="inlineStr">
         <is>
@@ -24607,13 +24063,11 @@
       </c>
       <c r="L274" t="inlineStr">
         <is>
-          <t>Merida</t>
-        </is>
-      </c>
-      <c r="M274" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M274" t="n">
+        <v>97305</v>
       </c>
       <c r="N274" t="inlineStr">
         <is>
@@ -24696,13 +24150,11 @@
       </c>
       <c r="L275" t="inlineStr">
         <is>
-          <t>Merida</t>
-        </is>
-      </c>
-      <c r="M275" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M275" t="n">
+        <v>97305</v>
       </c>
       <c r="N275" t="inlineStr">
         <is>
@@ -24785,13 +24237,11 @@
       </c>
       <c r="L276" t="inlineStr">
         <is>
-          <t>Merida</t>
-        </is>
-      </c>
-      <c r="M276" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M276" t="n">
+        <v>97305</v>
       </c>
       <c r="N276" t="inlineStr">
         <is>
@@ -24874,13 +24324,11 @@
       </c>
       <c r="L277" t="inlineStr">
         <is>
-          <t>Merida</t>
-        </is>
-      </c>
-      <c r="M277" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M277" t="n">
+        <v>97305</v>
       </c>
       <c r="N277" t="inlineStr">
         <is>
@@ -24963,13 +24411,11 @@
       </c>
       <c r="L278" t="inlineStr">
         <is>
-          <t>Merida</t>
-        </is>
-      </c>
-      <c r="M278" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M278" t="n">
+        <v>97305</v>
       </c>
       <c r="N278" t="inlineStr">
         <is>
@@ -25052,13 +24498,11 @@
       </c>
       <c r="L279" t="inlineStr">
         <is>
-          <t>Merida</t>
-        </is>
-      </c>
-      <c r="M279" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M279" t="n">
+        <v>97305</v>
       </c>
       <c r="N279" t="inlineStr">
         <is>
@@ -25141,13 +24585,11 @@
       </c>
       <c r="L280" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M280" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M280" t="n">
+        <v>97302</v>
       </c>
       <c r="N280" t="inlineStr">
         <is>
@@ -25230,13 +24672,11 @@
       </c>
       <c r="L281" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M281" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M281" t="n">
+        <v>97302</v>
       </c>
       <c r="N281" t="inlineStr">
         <is>
@@ -25319,13 +24759,11 @@
       </c>
       <c r="L282" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M282" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M282" t="n">
+        <v>97302</v>
       </c>
       <c r="N282" t="inlineStr">
         <is>
@@ -25404,13 +24842,11 @@
       </c>
       <c r="L283" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M283" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M283" t="n">
+        <v>97219</v>
       </c>
       <c r="N283" t="inlineStr">
         <is>
@@ -25470,13 +24906,11 @@
       </c>
       <c r="L284" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M284" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M284" t="n">
+        <v>97114</v>
       </c>
       <c r="N284" t="inlineStr">
         <is>
@@ -25536,13 +24970,11 @@
       </c>
       <c r="L285" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M285" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M285" t="n">
+        <v>97114</v>
       </c>
       <c r="N285" t="inlineStr">
         <is>
@@ -25627,13 +25059,11 @@
       </c>
       <c r="L286" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M286" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M286" t="n">
+        <v>97114</v>
       </c>
       <c r="N286" t="inlineStr">
         <is>
@@ -25693,13 +25123,11 @@
       </c>
       <c r="L287" t="inlineStr">
         <is>
-          <t>Mérida</t>
-        </is>
-      </c>
-      <c r="M287" t="inlineStr">
-        <is>
           <t>YUCATÁN</t>
         </is>
+      </c>
+      <c r="M287" t="n">
+        <v>97302</v>
       </c>
       <c r="N287" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
feat(arsenal): Registrar CZ P-10 C para Ricardo Soberanis (Credencial 230)
- Agregada nueva pistola CZ P-10 C a Excel (fila 283)
- Calibre: .40 S&W
- Matrícula: EP29710
- Folio SEDENA: A3912487
- Registrado en Firestore (ID: 8d1f8140)
- PDF subido a Firebase Storage
- Total armas Ricardo: 4
</commit_message>
<xml_diff>
--- a/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S287"/>
+  <dimension ref="A1:S288"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25890,39 +25890,39 @@
         </is>
       </c>
       <c r="C283" t="n">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>RAÚL CERVANTES CEBALLOS</t>
+          <t>RICARDO ANTONIO SOBERANIS GAMBOA</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
         <is>
-          <t>CECR890104HYNRBL02</t>
-        </is>
-      </c>
-      <c r="F283" s="4" t="inlineStr">
-        <is>
-          <t>'9993382222</t>
+          <t>SOGR701015HYNBMC04</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>'9993437376</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
         <is>
-          <t>rcervantes@live.com.mx</t>
+          <t>rsoberanis11@hotmail.com</t>
         </is>
       </c>
       <c r="H283" s="2" t="n">
-        <v>45835</v>
+        <v>45808</v>
       </c>
       <c r="I283" t="inlineStr">
         <is>
-          <t>C 13 POR 62 Y 64 655</t>
+          <t>Calle 23 S/N T.C. 50641</t>
         </is>
       </c>
       <c r="J283" t="inlineStr">
         <is>
-          <t>RESIDENCIAL PENSIONES</t>
+          <t>Colonia San Antonio Hool</t>
         </is>
       </c>
       <c r="K283" t="inlineStr">
@@ -25935,14 +25935,39 @@
           <t>YUCATÁN</t>
         </is>
       </c>
-      <c r="M283" s="4" t="inlineStr">
-        <is>
-          <t>'97219</t>
+      <c r="M283" t="inlineStr">
+        <is>
+          <t>'97302</t>
         </is>
       </c>
       <c r="N283" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>PISTOLA</t>
+        </is>
+      </c>
+      <c r="O283" t="inlineStr">
+        <is>
+          <t>.40 S&amp;W</t>
+        </is>
+      </c>
+      <c r="P283" t="inlineStr">
+        <is>
+          <t>CZ</t>
+        </is>
+      </c>
+      <c r="Q283" t="inlineStr">
+        <is>
+          <t>P-10 C</t>
+        </is>
+      </c>
+      <c r="R283" t="inlineStr">
+        <is>
+          <t>EP29710</t>
+        </is>
+      </c>
+      <c r="S283" t="inlineStr">
+        <is>
+          <t>A3912487</t>
         </is>
       </c>
     </row>
@@ -25956,39 +25981,39 @@
         </is>
       </c>
       <c r="C284" t="n">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D284" t="inlineStr">
         <is>
-          <t>RICARDO DANIEL FERNÁNDEZ PÉREZ</t>
+          <t>RAÚL CERVANTES CEBALLOS</t>
         </is>
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>FEPR920403HYNRRC06</t>
+          <t>CECR890104HYNRBL02</t>
         </is>
       </c>
       <c r="F284" s="4" t="inlineStr">
         <is>
-          <t>'9991639981</t>
+          <t>'9993382222</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
         <is>
-          <t>richfer0304@gmail.com</t>
+          <t>rcervantes@live.com.mx</t>
         </is>
       </c>
       <c r="H284" s="2" t="n">
-        <v>45864</v>
+        <v>45835</v>
       </c>
       <c r="I284" t="inlineStr">
         <is>
-          <t>C. 37-A # 311 X 24</t>
+          <t>C 13 POR 62 Y 64 655</t>
         </is>
       </c>
       <c r="J284" t="inlineStr">
         <is>
-          <t>FRACC. MONTEALBAN</t>
+          <t>RESIDENCIAL PENSIONES</t>
         </is>
       </c>
       <c r="K284" t="inlineStr">
@@ -26003,7 +26028,7 @@
       </c>
       <c r="M284" s="4" t="inlineStr">
         <is>
-          <t>'97114</t>
+          <t>'97219</t>
         </is>
       </c>
       <c r="N284" t="inlineStr">
@@ -26022,26 +26047,26 @@
         </is>
       </c>
       <c r="C285" t="n">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>RICARDO MANUEL FERNÁNDEZ QUIJANO</t>
+          <t>RICARDO DANIEL FERNÁNDEZ PÉREZ</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>FEQR591020HCCRJC07</t>
+          <t>FEPR920403HYNRRC06</t>
         </is>
       </c>
       <c r="F285" s="4" t="inlineStr">
         <is>
-          <t>'9999473043</t>
+          <t>'9991639981</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
         <is>
-          <t>richfer1020@gmail.com</t>
+          <t>richfer0304@gmail.com</t>
         </is>
       </c>
       <c r="H285" s="2" t="n">
@@ -26074,32 +26099,7 @@
       </c>
       <c r="N285" t="inlineStr">
         <is>
-          <t>PISTOLA</t>
-        </is>
-      </c>
-      <c r="O285" t="inlineStr">
-        <is>
-          <t>0.380"</t>
-        </is>
-      </c>
-      <c r="P285" t="inlineStr">
-        <is>
-          <t>GLOCK</t>
-        </is>
-      </c>
-      <c r="Q285" s="4" t="inlineStr">
-        <is>
-          <t>25</t>
-        </is>
-      </c>
-      <c r="R285" s="3" t="inlineStr">
-        <is>
-          <t>UDV639</t>
-        </is>
-      </c>
-      <c r="S285" t="inlineStr">
-        <is>
-          <t>B347208</t>
+          <t>0</t>
         </is>
       </c>
     </row>
@@ -26113,39 +26113,39 @@
         </is>
       </c>
       <c r="C286" t="n">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>YAEL ROMERO DE DIOS</t>
+          <t>RICARDO MANUEL FERNÁNDEZ QUIJANO</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
         <is>
-          <t>RODY940625HYNMSL01</t>
+          <t>FEQR591020HCCRJC07</t>
         </is>
       </c>
       <c r="F286" s="4" t="inlineStr">
         <is>
-          <t>'9995287779</t>
+          <t>'9999473043</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>licyaelromero@gmail.com</t>
+          <t>richfer1020@gmail.com</t>
         </is>
       </c>
       <c r="H286" s="2" t="n">
-        <v>45899</v>
+        <v>45864</v>
       </c>
       <c r="I286" t="inlineStr">
         <is>
-          <t>Calle 111 No 514 x 132 y 134A</t>
+          <t>C. 37-A # 311 X 24</t>
         </is>
       </c>
       <c r="J286" t="inlineStr">
         <is>
-          <t>Fraccionamiento los Héroes.</t>
+          <t>FRACC. MONTEALBAN</t>
         </is>
       </c>
       <c r="K286" t="inlineStr">
@@ -26165,7 +26165,32 @@
       </c>
       <c r="N286" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>PISTOLA</t>
+        </is>
+      </c>
+      <c r="O286" t="inlineStr">
+        <is>
+          <t>0.380"</t>
+        </is>
+      </c>
+      <c r="P286" t="inlineStr">
+        <is>
+          <t>GLOCK</t>
+        </is>
+      </c>
+      <c r="Q286" s="4" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="R286" s="3" t="inlineStr">
+        <is>
+          <t>UDV639</t>
+        </is>
+      </c>
+      <c r="S286" t="inlineStr">
+        <is>
+          <t>B347208</t>
         </is>
       </c>
     </row>
@@ -26179,57 +26204,123 @@
         </is>
       </c>
       <c r="C287" t="n">
+        <v>234</v>
+      </c>
+      <c r="D287" t="inlineStr">
+        <is>
+          <t>YAEL ROMERO DE DIOS</t>
+        </is>
+      </c>
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>RODY940625HYNMSL01</t>
+        </is>
+      </c>
+      <c r="F287" s="4" t="inlineStr">
+        <is>
+          <t>'9995287779</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>licyaelromero@gmail.com</t>
+        </is>
+      </c>
+      <c r="H287" s="2" t="n">
+        <v>45899</v>
+      </c>
+      <c r="I287" t="inlineStr">
+        <is>
+          <t>Calle 111 No 514 x 132 y 134A</t>
+        </is>
+      </c>
+      <c r="J287" t="inlineStr">
+        <is>
+          <t>Fraccionamiento los Héroes.</t>
+        </is>
+      </c>
+      <c r="K287" t="inlineStr">
+        <is>
+          <t>Mérida</t>
+        </is>
+      </c>
+      <c r="L287" t="inlineStr">
+        <is>
+          <t>YUCATÁN</t>
+        </is>
+      </c>
+      <c r="M287" s="4" t="inlineStr">
+        <is>
+          <t>'97114</t>
+        </is>
+      </c>
+      <c r="N287" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="n">
+        <v>738</v>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t>CALLE 50 No. 531-E x 69 y 71, CENTRO, 97000 MÉRIDA, YUC.</t>
+        </is>
+      </c>
+      <c r="C288" t="n">
         <v>235</v>
       </c>
-      <c r="D287" t="inlineStr">
+      <c r="D288" t="inlineStr">
         <is>
           <t>AIMEE GOMEZ MENDOZA</t>
         </is>
       </c>
-      <c r="E287" t="inlineStr">
+      <c r="E288" t="inlineStr">
         <is>
           <t>GOMA940118MVZMNM00</t>
         </is>
       </c>
-      <c r="F287" s="4" t="inlineStr">
+      <c r="F288" s="4" t="inlineStr">
         <is>
           <t>'9997300081</t>
         </is>
       </c>
-      <c r="G287" t="inlineStr">
+      <c r="G288" t="inlineStr">
         <is>
           <t>aimeegomez615@gmail.com</t>
         </is>
       </c>
-      <c r="H287" s="2" t="n">
+      <c r="H288" s="2" t="n">
         <v>46006</v>
       </c>
-      <c r="I287" t="inlineStr">
+      <c r="I288" t="inlineStr">
         <is>
           <t>C 63 D POR 88 TAB 42155</t>
         </is>
       </c>
-      <c r="J287" t="inlineStr">
+      <c r="J288" t="inlineStr">
         <is>
           <t>LOC DZITYA</t>
         </is>
       </c>
-      <c r="K287" t="inlineStr">
+      <c r="K288" t="inlineStr">
         <is>
           <t>Mérida</t>
         </is>
       </c>
-      <c r="L287" t="inlineStr">
+      <c r="L288" t="inlineStr">
         <is>
           <t>YUCATÁN</t>
         </is>
       </c>
-      <c r="M287" s="4" t="inlineStr">
+      <c r="M288" s="4" t="inlineStr">
         <is>
           <t>'97302</t>
         </is>
       </c>
-      <c r="N287" t="inlineStr">
+      <c r="N288" t="inlineStr">
         <is>
           <t>0</t>
         </is>

</xml_diff>

<commit_message>
fix(arsenal): calibre correcto CZ P-10 C (.380" ACP) + lección en copilot-instructions
- Corregir calibre en Excel fila 283: .40 S&W → .380" ACP
- Corregir calibre en Firestore ID 8d1f8140: .40 S&W → .380" ACP
- Agregar marca: CESKA ZBROJOVKA
- LECCIÓN: NUNCA asumir calibres sin OCR - máximo legal civiles es .380" ACP (SEDENA Art. 50)
- Ricardo Soberanis: PISTOLA CZ P-10 C (matricula EP29710, folio A3912487)
</commit_message>
<xml_diff>
--- a/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -25947,12 +25947,12 @@
       </c>
       <c r="O283" t="inlineStr">
         <is>
-          <t>.40 S&amp;W</t>
+          <t>.380"</t>
         </is>
       </c>
       <c r="P283" t="inlineStr">
         <is>
-          <t>CZ</t>
+          <t>CESKA ZBROJOVKA</t>
         </is>
       </c>
       <c r="Q283" t="inlineStr">

</xml_diff>

<commit_message>
fix(data): Sincronización final Excel + Firestore - Restauradas transferencias Gardoni ↔ Arechiga
</commit_message>
<xml_diff>
--- a/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -25548,6 +25548,11 @@
           <t>jrgardoni@gmail.com</t>
         </is>
       </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>jrgardoni@gmail.com</t>
+        </is>
+      </c>
       <c r="N280" t="inlineStr">
         <is>
           <t>PISTOLA</t>
@@ -25593,6 +25598,11 @@
           <t>jrgardoni@gmail.com</t>
         </is>
       </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>jrgardoni@gmail.com</t>
+        </is>
+      </c>
       <c r="N281" t="inlineStr">
         <is>
           <t>RIFLE</t>
@@ -25638,6 +25648,11 @@
           <t>jrgardoni@gmail.com</t>
         </is>
       </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>jrgardoni@gmail.com</t>
+        </is>
+      </c>
       <c r="N282" t="inlineStr">
         <is>
           <t>RIFLE</t>
@@ -25683,6 +25698,11 @@
           <t>jrgardoni@gmail.com</t>
         </is>
       </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>jrgardoni@gmail.com</t>
+        </is>
+      </c>
       <c r="N283" t="inlineStr">
         <is>
           <t>RIFLE</t>
@@ -25728,6 +25748,11 @@
           <t>jrgardoni@gmail.com</t>
         </is>
       </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>jrgardoni@gmail.com</t>
+        </is>
+      </c>
       <c r="N284" t="inlineStr">
         <is>
           <t>PISTOLA</t>
@@ -25773,6 +25798,11 @@
           <t>jrgardoni@gmail.com</t>
         </is>
       </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>jrgardoni@gmail.com</t>
+        </is>
+      </c>
       <c r="N285" t="inlineStr">
         <is>
           <t>PISTOLA</t>
@@ -25818,6 +25848,11 @@
           <t>jrgardoni@gmail.com</t>
         </is>
       </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>jrgardoni@gmail.com</t>
+        </is>
+      </c>
       <c r="N286" t="inlineStr">
         <is>
           <t>PISTOLA</t>
@@ -25863,6 +25898,11 @@
           <t>arechiga@jogarplastics.com</t>
         </is>
       </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>arechiga@jogarplastics.com</t>
+        </is>
+      </c>
       <c r="N287" t="inlineStr">
         <is>
           <t>PISTOLA</t>
@@ -25908,6 +25948,11 @@
           <t>arechiga@jogarplastics.com</t>
         </is>
       </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>arechiga@jogarplastics.com</t>
+        </is>
+      </c>
       <c r="N288" t="inlineStr">
         <is>
           <t>PISTOLA</t>
@@ -25949,6 +25994,11 @@
         </is>
       </c>
       <c r="E289" t="inlineStr">
+        <is>
+          <t>arechiga@jogarplastics.com</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
         <is>
           <t>arechiga@jogarplastics.com</t>
         </is>

</xml_diff>

<commit_message>
feat(arsenal): Agregar 4 armas nuevas a Celestino Sánchez (Credencial 183)
- RIFLE Winchester 9422 (.22" L.R., F11281, A3917581)
- PISTOLA CZ P-07 (.380" AUTO, D207727, A3747924)
- PISTOLA CZ P-10 C (.380" AUTO, CP18665, A3747922)
- PISTOLA SIG SAUER P250 (.380" AUTO, 57C048858, B596607)

Total arsenal Celestino: 5 armas (1 ESCOPETA + 1 RIFLE + 3 PISTOLAS)
Excel y Firestore sincronizados.
</commit_message>
<xml_diff>
--- a/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S289"/>
+  <dimension ref="A1:S293"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26034,6 +26034,186 @@
         </is>
       </c>
     </row>
+    <row r="290">
+      <c r="C290" t="n">
+        <v>183</v>
+      </c>
+      <c r="D290" t="inlineStr">
+        <is>
+          <t>CELESTINO SANCHEZ FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>tinosanchezf@yahoo.com.mx</t>
+        </is>
+      </c>
+      <c r="N290" t="inlineStr">
+        <is>
+          <t>RIFLE</t>
+        </is>
+      </c>
+      <c r="O290" t="inlineStr">
+        <is>
+          <t>.22" L.R.</t>
+        </is>
+      </c>
+      <c r="P290" t="inlineStr">
+        <is>
+          <t>WINCHESTER</t>
+        </is>
+      </c>
+      <c r="Q290" t="inlineStr">
+        <is>
+          <t>9422</t>
+        </is>
+      </c>
+      <c r="R290" t="inlineStr">
+        <is>
+          <t>F11281</t>
+        </is>
+      </c>
+      <c r="S290" t="inlineStr">
+        <is>
+          <t>A3917581</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="C291" t="n">
+        <v>183</v>
+      </c>
+      <c r="D291" t="inlineStr">
+        <is>
+          <t>CELESTINO SANCHEZ FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>tinosanchezf@yahoo.com.mx</t>
+        </is>
+      </c>
+      <c r="N291" t="inlineStr">
+        <is>
+          <t>PISTOLA</t>
+        </is>
+      </c>
+      <c r="O291" t="inlineStr">
+        <is>
+          <t>.380" AUTO</t>
+        </is>
+      </c>
+      <c r="P291" t="inlineStr">
+        <is>
+          <t>CESKA ZBROJOVKA</t>
+        </is>
+      </c>
+      <c r="Q291" t="inlineStr">
+        <is>
+          <t>CZ P-07</t>
+        </is>
+      </c>
+      <c r="R291" t="inlineStr">
+        <is>
+          <t>D207727</t>
+        </is>
+      </c>
+      <c r="S291" t="inlineStr">
+        <is>
+          <t>A3747924</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="C292" t="n">
+        <v>183</v>
+      </c>
+      <c r="D292" t="inlineStr">
+        <is>
+          <t>CELESTINO SANCHEZ FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>tinosanchezf@yahoo.com.mx</t>
+        </is>
+      </c>
+      <c r="N292" t="inlineStr">
+        <is>
+          <t>PISTOLA</t>
+        </is>
+      </c>
+      <c r="O292" t="inlineStr">
+        <is>
+          <t>.380" AUTO</t>
+        </is>
+      </c>
+      <c r="P292" t="inlineStr">
+        <is>
+          <t>CESKA ZBROJOVKA</t>
+        </is>
+      </c>
+      <c r="Q292" t="inlineStr">
+        <is>
+          <t>CZ P-10 C</t>
+        </is>
+      </c>
+      <c r="R292" t="inlineStr">
+        <is>
+          <t>CP18665</t>
+        </is>
+      </c>
+      <c r="S292" t="inlineStr">
+        <is>
+          <t>A3747922</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="C293" t="n">
+        <v>183</v>
+      </c>
+      <c r="D293" t="inlineStr">
+        <is>
+          <t>CELESTINO SANCHEZ FERNANDEZ</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>tinosanchezf@yahoo.com.mx</t>
+        </is>
+      </c>
+      <c r="N293" t="inlineStr">
+        <is>
+          <t>PISTOLA</t>
+        </is>
+      </c>
+      <c r="O293" t="inlineStr">
+        <is>
+          <t>.380" AUTO</t>
+        </is>
+      </c>
+      <c r="P293" t="inlineStr">
+        <is>
+          <t>SIG SAUER</t>
+        </is>
+      </c>
+      <c r="Q293" t="inlineStr">
+        <is>
+          <t>P250</t>
+        </is>
+      </c>
+      <c r="R293" t="inlineStr">
+        <is>
+          <t>57C048858</t>
+        </is>
+      </c>
+      <c r="S293" t="inlineStr">
+        <is>
+          <t>B596607</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: agregar credencial 236 - Luis Fernando Guillermo Gamboa al Excel
</commit_message>
<xml_diff>
--- a/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
+++ b/socios/FUENTE_DE_VERDAD_CLUB_738_ENERO_2026.xlsx
@@ -434,7 +434,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S293"/>
+  <dimension ref="A1:S294"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -26214,6 +26214,42 @@
         </is>
       </c>
     </row>
+    <row r="294">
+      <c r="B294" t="inlineStr">
+        <is>
+          <t>Calle 32 x 9 Cedro, Tablaje 23222, Loc. Tixcuytun, Mérida, YUCATÁN CP97305</t>
+        </is>
+      </c>
+      <c r="C294" t="n">
+        <v>236</v>
+      </c>
+      <c r="D294" t="inlineStr">
+        <is>
+          <t>LUIS FERNANDO GUILLERMO GAMBOA</t>
+        </is>
+      </c>
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>GUGL750204HYNLMS04</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>9992420621</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>oso.guigam@gmail.com</t>
+        </is>
+      </c>
+      <c r="H294" s="2" t="n">
+        <v>46030</v>
+      </c>
+      <c r="N294" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>